<commit_message>
updated after review of variables
</commit_message>
<xml_diff>
--- a/Feb 10 from Delvin/CA_variable_check_accepted_ranges.xlsx
+++ b/Feb 10 from Delvin/CA_variable_check_accepted_ranges.xlsx
@@ -5,33 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/delvin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ivanics/Desktop/GitHub/MLA-International-registries/Feb 10 from Delvin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5971AC7C-FC17-6A4E-BA34-5EF526D52D0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E1C258-B93D-D14F-920A-1BF82C3CE703}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16940" yWindow="6580" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19880" yWindow="500" windowWidth="27040" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ca_usable_missingness_post_proc" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="96">
   <si>
     <t>variable</t>
   </si>
@@ -289,6 +278,36 @@
   </si>
   <si>
     <t>no cutoff</t>
+  </si>
+  <si>
+    <t>Too many missing</t>
+  </si>
+  <si>
+    <t>A lot of missing but very important variable</t>
+  </si>
+  <si>
+    <t>Too many missing (remind me its &gt;25% right?)</t>
+  </si>
+  <si>
+    <t>Cutoff?</t>
+  </si>
+  <si>
+    <t>Keep</t>
+  </si>
+  <si>
+    <t>0 or 1</t>
+  </si>
+  <si>
+    <t>2008 to 2018</t>
+  </si>
+  <si>
+    <t>no cutoff (identifier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 to 210 </t>
+  </si>
+  <si>
+    <t>kg</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1161,7 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1151,6 +1170,7 @@
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="37.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1189,6 +1209,9 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
@@ -1209,6 +1232,9 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
       <c r="F3" t="s">
         <v>69</v>
       </c>
@@ -1232,6 +1258,9 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
       <c r="F4" t="s">
         <v>70</v>
       </c>
@@ -1249,6 +1278,9 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
       <c r="F5" t="s">
         <v>71</v>
       </c>
@@ -1266,6 +1298,9 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
       <c r="F6" t="s">
         <v>72</v>
       </c>
@@ -1283,6 +1318,9 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1297,6 +1335,9 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1311,6 +1352,9 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
+      <c r="E9" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1325,6 +1369,9 @@
       <c r="D10" t="s">
         <v>11</v>
       </c>
+      <c r="E10" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1339,6 +1386,9 @@
       <c r="D11" t="s">
         <v>11</v>
       </c>
+      <c r="E11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1353,6 +1403,9 @@
       <c r="D12" t="s">
         <v>11</v>
       </c>
+      <c r="E12" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1367,6 +1420,9 @@
       <c r="D13" t="s">
         <v>11</v>
       </c>
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1381,6 +1437,9 @@
       <c r="D14" t="s">
         <v>11</v>
       </c>
+      <c r="E14" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1395,6 +1454,9 @@
       <c r="D15" t="s">
         <v>11</v>
       </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1409,6 +1471,9 @@
       <c r="D16" t="s">
         <v>5</v>
       </c>
+      <c r="E16" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1423,6 +1488,9 @@
       <c r="D17" t="s">
         <v>11</v>
       </c>
+      <c r="E17" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1437,6 +1505,9 @@
       <c r="D18" t="s">
         <v>5</v>
       </c>
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
       <c r="F18" t="s">
         <v>73</v>
       </c>
@@ -1454,6 +1525,9 @@
       <c r="D19" t="s">
         <v>11</v>
       </c>
+      <c r="E19" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -1468,6 +1542,9 @@
       <c r="D20" t="s">
         <v>11</v>
       </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1482,6 +1559,9 @@
       <c r="D21" t="s">
         <v>11</v>
       </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1496,6 +1576,9 @@
       <c r="D22" t="s">
         <v>11</v>
       </c>
+      <c r="E22" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1510,6 +1593,9 @@
       <c r="D23" t="s">
         <v>5</v>
       </c>
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1524,6 +1610,9 @@
       <c r="D24" t="s">
         <v>11</v>
       </c>
+      <c r="E24" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1538,6 +1627,9 @@
       <c r="D25" t="s">
         <v>5</v>
       </c>
+      <c r="E25" t="s">
+        <v>90</v>
+      </c>
       <c r="F25" t="s">
         <v>74</v>
       </c>
@@ -1555,6 +1647,9 @@
       <c r="D26" t="s">
         <v>11</v>
       </c>
+      <c r="E26" t="s">
+        <v>90</v>
+      </c>
       <c r="F26" t="s">
         <v>75</v>
       </c>
@@ -1575,6 +1670,9 @@
       <c r="D27" t="s">
         <v>11</v>
       </c>
+      <c r="E27" t="s">
+        <v>90</v>
+      </c>
       <c r="F27" t="s">
         <v>77</v>
       </c>
@@ -1595,6 +1693,9 @@
       <c r="D28" t="s">
         <v>11</v>
       </c>
+      <c r="E28" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1609,6 +1710,9 @@
       <c r="D29" t="s">
         <v>11</v>
       </c>
+      <c r="E29" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1623,6 +1727,9 @@
       <c r="D30" t="s">
         <v>5</v>
       </c>
+      <c r="E30" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1637,6 +1744,9 @@
       <c r="D31" t="s">
         <v>11</v>
       </c>
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1651,6 +1761,9 @@
       <c r="D32" t="s">
         <v>11</v>
       </c>
+      <c r="E32" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -1665,6 +1778,9 @@
       <c r="D33" t="s">
         <v>5</v>
       </c>
+      <c r="E33" t="s">
+        <v>90</v>
+      </c>
       <c r="F33" t="s">
         <v>74</v>
       </c>
@@ -1682,6 +1798,9 @@
       <c r="D34" t="s">
         <v>5</v>
       </c>
+      <c r="E34" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -1696,6 +1815,9 @@
       <c r="D35" t="s">
         <v>11</v>
       </c>
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
       <c r="F35" t="s">
         <v>75</v>
       </c>
@@ -1713,6 +1835,9 @@
       <c r="D36" t="s">
         <v>5</v>
       </c>
+      <c r="E36" t="s">
+        <v>90</v>
+      </c>
       <c r="F36" s="2" t="s">
         <v>85</v>
       </c>
@@ -1730,6 +1855,9 @@
       <c r="D37" t="s">
         <v>5</v>
       </c>
+      <c r="E37" t="s">
+        <v>90</v>
+      </c>
       <c r="F37" t="s">
         <v>79</v>
       </c>
@@ -1747,6 +1875,9 @@
       <c r="D38" t="s">
         <v>5</v>
       </c>
+      <c r="E38" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -1761,6 +1892,9 @@
       <c r="D39" t="s">
         <v>5</v>
       </c>
+      <c r="E39" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -1775,6 +1909,9 @@
       <c r="D40" t="s">
         <v>5</v>
       </c>
+      <c r="E40" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -1789,6 +1926,9 @@
       <c r="D41" t="s">
         <v>5</v>
       </c>
+      <c r="E41" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -1803,6 +1943,9 @@
       <c r="D42" t="s">
         <v>5</v>
       </c>
+      <c r="E42" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -1817,6 +1960,9 @@
       <c r="D43" t="s">
         <v>5</v>
       </c>
+      <c r="E43" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -1831,6 +1977,9 @@
       <c r="D44" t="s">
         <v>5</v>
       </c>
+      <c r="E44" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -1845,6 +1994,9 @@
       <c r="D45" t="s">
         <v>5</v>
       </c>
+      <c r="E45" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -1859,6 +2011,9 @@
       <c r="D46" t="s">
         <v>5</v>
       </c>
+      <c r="E46" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -1873,6 +2028,9 @@
       <c r="D47" t="s">
         <v>5</v>
       </c>
+      <c r="E47" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -1887,8 +2045,11 @@
       <c r="D48" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1901,8 +2062,17 @@
       <c r="D49" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" t="s">
+        <v>94</v>
+      </c>
+      <c r="G49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1915,8 +2085,11 @@
       <c r="D50" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1929,8 +2102,14 @@
       <c r="D51" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>90</v>
+      </c>
+      <c r="F51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1943,8 +2122,14 @@
       <c r="D52" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>90</v>
+      </c>
+      <c r="F52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -1957,8 +2142,11 @@
       <c r="D53" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -1971,8 +2159,11 @@
       <c r="D54" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -1985,8 +2176,11 @@
       <c r="D55" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -1999,8 +2193,14 @@
       <c r="D56" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>90</v>
+      </c>
+      <c r="F56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -2013,8 +2213,11 @@
       <c r="D57" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -2027,8 +2230,14 @@
       <c r="D58" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E58" t="s">
+        <v>90</v>
+      </c>
+      <c r="F58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -2041,11 +2250,14 @@
       <c r="D59" t="s">
         <v>5</v>
       </c>
+      <c r="E59" t="s">
+        <v>90</v>
+      </c>
       <c r="F59" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -2058,8 +2270,14 @@
       <c r="D60" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>90</v>
+      </c>
+      <c r="F60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -2072,8 +2290,14 @@
       <c r="D61" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>90</v>
+      </c>
+      <c r="F61" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -2086,8 +2310,11 @@
       <c r="D62" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2100,8 +2327,11 @@
       <c r="D63" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -2113,6 +2343,9 @@
       </c>
       <c r="D64" t="s">
         <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>